<commit_message>
B Binning Bettered Bigly
</commit_message>
<xml_diff>
--- a/C6/PartBData.xlsx
+++ b/C6/PartBData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\GitHub\24321-A4\C6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAD6A39B-5C9B-4F96-820A-C5D359ED496F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC72D1BF-1F1E-45C7-8E11-C292CB56926A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25560" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{524206DC-CDE0-4926-96B1-4293AC0B41F9}"/>
   </bookViews>
@@ -522,7 +522,7 @@
         <v>-6.8899999999999739E-2</v>
       </c>
       <c r="J2">
-        <v>0.27644941667066897</v>
+        <v>-0.12245117018844072</v>
       </c>
       <c r="K2">
         <v>2.5462055831416416E-2</v>
@@ -531,7 +531,7 @@
         <v>3.8014303219283041E-3</v>
       </c>
       <c r="M2">
-        <v>-0.56313319240686954</v>
+        <v>-0.55313604614502221</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>-5.7599999999999874E-2</v>
       </c>
       <c r="J3">
-        <v>0.29389410469521127</v>
+        <v>-0.12245117018844072</v>
       </c>
       <c r="K3">
         <v>2.5462055831416416E-2</v>
@@ -572,7 +572,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M3">
-        <v>-0.4826927695975568</v>
+        <v>-0.55313604614502221</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>-9.1900000000000315E-2</v>
       </c>
       <c r="J4">
-        <v>0.23490254503609925</v>
+        <v>-0.12245117018844072</v>
       </c>
       <c r="K4">
         <v>2.5462055831416416E-2</v>
@@ -613,7 +613,7 @@
         <v>3.8014303219283041E-3</v>
       </c>
       <c r="M4">
-        <v>-0.75111669640336265</v>
+        <v>-0.55313604614502221</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>-5.7800000000000296E-2</v>
       </c>
       <c r="J5">
-        <v>0.29352252383303395</v>
+        <v>-0.12245117018844072</v>
       </c>
       <c r="K5">
         <v>2.5462055831416416E-2</v>
@@ -654,7 +654,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M5">
-        <v>-0.48436878615866286</v>
+        <v>-0.55313604614502221</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>-5.7799999999999851E-2</v>
       </c>
       <c r="J6">
-        <v>0.29352252383303479</v>
+        <v>-0.12245117018844072</v>
       </c>
       <c r="K6">
         <v>2.5462055831416416E-2</v>
@@ -695,7 +695,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M6">
-        <v>-0.48436878615865925</v>
+        <v>-0.55313604614502221</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>-1.0599999999999721E-2</v>
       </c>
       <c r="J7">
-        <v>0.37487163918659028</v>
+        <v>-3.6955121270099381E-2</v>
       </c>
       <c r="K7">
         <v>3.1618652440573436E-2</v>
@@ -736,7 +736,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M7">
-        <v>-0.1138263182074616</v>
+        <v>-0.1617143664617105</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>-2.1999999999999797E-2</v>
       </c>
       <c r="J8">
-        <v>0.3485880114899394</v>
+        <v>-3.6955121270099381E-2</v>
       </c>
       <c r="K8">
         <v>3.1618652440573436E-2</v>
@@ -777,7 +777,7 @@
         <v>3.9201744307436788E-3</v>
       </c>
       <c r="M8">
-        <v>-0.22956319365554023</v>
+        <v>-0.1617143664617105</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>-3.3399999999999874E-2</v>
       </c>
       <c r="J9">
-        <v>0.31886590456465547</v>
+        <v>-3.6955121270099381E-2</v>
       </c>
       <c r="K9">
         <v>3.1618652440573436E-2</v>
@@ -818,7 +818,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M9">
-        <v>-0.3586602856725758</v>
+        <v>-0.1617143664617105</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>-1.0600000000000165E-2</v>
       </c>
       <c r="J10">
-        <v>0.37487163918658922</v>
+        <v>-3.6955121270099381E-2</v>
       </c>
       <c r="K10">
         <v>3.1618652440573436E-2</v>
@@ -859,7 +859,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M10">
-        <v>-0.11382631820746636</v>
+        <v>-0.1617143664617105</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>6.9999999999970086E-4</v>
       </c>
       <c r="J11">
-        <v>0.40257416423198045</v>
+        <v>-3.6955121270099381E-2</v>
       </c>
       <c r="K11">
         <v>3.1618652440573436E-2</v>
@@ -900,7 +900,7 @@
         <v>3.9201744307436788E-3</v>
       </c>
       <c r="M11">
-        <v>7.3042834344914081E-3</v>
+        <v>-0.1617143664617105</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>3.620000000000001E-2</v>
       </c>
       <c r="J12">
-        <v>0.52878863249754637</v>
+        <v>8.6352420326484339E-2</v>
       </c>
       <c r="K12">
         <v>2.9498935557444494E-2</v>
@@ -941,7 +941,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M12">
-        <v>0.53633741165374271</v>
+        <v>0.36291003389004739</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>2.50999999999999E-2</v>
       </c>
       <c r="J13">
-        <v>0.48621338180137486</v>
+        <v>8.6352420326484339E-2</v>
       </c>
       <c r="K13">
         <v>2.9498935557444494E-2</v>
@@ -982,7 +982,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M13">
-        <v>0.35936956693578165</v>
+        <v>0.36291003389004739</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>2.4799999999999933E-2</v>
       </c>
       <c r="J14">
-        <v>0.48205309221503956</v>
+        <v>8.6352420326484339E-2</v>
       </c>
       <c r="K14">
         <v>2.9498935557444494E-2</v>
@@ -1023,7 +1023,7 @@
         <v>4.0650106703421542E-3</v>
       </c>
       <c r="M14">
-        <v>0.34333775225882479</v>
+        <v>0.36291003389004739</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>1.3299999999999867E-2</v>
       </c>
       <c r="J15">
-        <v>0.44611031136981966</v>
+        <v>8.6352420326484339E-2</v>
       </c>
       <c r="K15">
         <v>2.9498935557444494E-2</v>
@@ -1064,7 +1064,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M15">
-        <v>0.19042291793808236</v>
+        <v>0.36291003389004739</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>2.50999999999999E-2</v>
       </c>
       <c r="J16">
-        <v>0.49314364875889316</v>
+        <v>8.6352420326484339E-2</v>
       </c>
       <c r="K16">
         <v>2.9498935557444494E-2</v>
@@ -1105,7 +1105,7 @@
         <v>4.1197123055157318E-3</v>
       </c>
       <c r="M16">
-        <v>0.38508252066380549</v>
+        <v>0.36291003389004739</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>4.9019999999999953E-2</v>
       </c>
       <c r="J17">
-        <v>0.65824995061282188</v>
+        <v>0.2930490535893206</v>
       </c>
       <c r="K17">
         <v>3.2597424038735168E-2</v>
@@ -1146,7 +1146,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M17">
-        <v>1.0305874973167799</v>
+        <v>1.1735914988824423</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>6.0390000000000055E-2</v>
       </c>
       <c r="J18">
-        <v>0.71793910075632461</v>
+        <v>0.2930490535893206</v>
       </c>
       <c r="K18">
         <v>3.2597424038735168E-2</v>
@@ -1187,7 +1187,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M18">
-        <v>1.2696282938180428</v>
+        <v>1.1735914988824423</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
         <v>6.0339999999999949E-2</v>
       </c>
       <c r="J19">
-        <v>0.71767661548744321</v>
+        <v>0.2930490535893206</v>
       </c>
       <c r="K19">
         <v>3.2597424038735168E-2</v>
@@ -1228,7 +1228,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M19">
-        <v>1.2685771029803043</v>
+        <v>1.1735914988824423</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>6.0339999999999949E-2</v>
       </c>
       <c r="J20">
-        <v>0.71767661548744321</v>
+        <v>0.2930490535893206</v>
       </c>
       <c r="K20">
         <v>3.2597424038735168E-2</v>
@@ -1269,7 +1269,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M20">
-        <v>1.2685771029803043</v>
+        <v>1.1735914988824423</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1301,7 +1301,7 @@
         <v>4.9019999999999953E-2</v>
       </c>
       <c r="J21">
-        <v>0.65824995061282188</v>
+        <v>0.2930490535893206</v>
       </c>
       <c r="K21">
         <v>3.2597424038735168E-2</v>
@@ -1310,7 +1310,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M21">
-        <v>1.0305874973167799</v>
+        <v>1.1735914988824423</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
         <v>7.2720000000000007E-2</v>
       </c>
       <c r="J22">
-        <v>1.0268642249716415</v>
+        <v>0.66775476882801921</v>
       </c>
       <c r="K22">
         <v>7.7485692283733046E-2</v>
@@ -1351,7 +1351,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M22">
-        <v>2.3627058129213583</v>
+        <v>2.5280109074748784</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>8.4100000000000008E-2</v>
       </c>
       <c r="J23">
-        <v>1.1248203029118773</v>
+        <v>0.66775476882801921</v>
       </c>
       <c r="K23">
         <v>7.7485692283733046E-2</v>
@@ -1392,7 +1392,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M23">
-        <v>2.7324471791348492</v>
+        <v>2.5280109074748784</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>7.2700000000000042E-2</v>
       </c>
       <c r="J24">
-        <v>1.0266920701773707</v>
+        <v>0.66775476882801921</v>
       </c>
       <c r="K24">
         <v>7.7485692283733046E-2</v>
@@ -1433,7 +1433,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M24">
-        <v>2.3620560038418983</v>
+        <v>2.5280109074748784</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>7.2720000000000007E-2</v>
       </c>
       <c r="J25">
-        <v>0.99035151057478776</v>
+        <v>0.66775476882801921</v>
       </c>
       <c r="K25">
         <v>7.7485692283733046E-2</v>
@@ -1474,7 +1474,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M25">
-        <v>2.2411638685625004</v>
+        <v>2.5280109074748784</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>9.5449999999999979E-2</v>
       </c>
       <c r="J26">
-        <v>1.1745927005146708</v>
+        <v>0.66775476882801921</v>
       </c>
       <c r="K26">
         <v>7.7485692283733046E-2</v>
@@ -1515,7 +1515,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M26">
-        <v>2.9416816729137869</v>
+        <v>2.5280109074748784</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>0.10764800000000001</v>
       </c>
       <c r="J27">
-        <v>2.0481462656941347</v>
+        <v>1.5177064067270183</v>
       </c>
       <c r="K27">
         <v>0.14454722515165275</v>
@@ -1556,7 +1556,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M27">
-        <v>5.7905446921186572</v>
+        <v>5.3459621777023081</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>8.4878999999999982E-2</v>
       </c>
       <c r="J28">
-        <v>1.6997335097272233</v>
+        <v>1.5177064067270183</v>
       </c>
       <c r="K28">
         <v>0.14454722515165275</v>
@@ -1597,7 +1597,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M28">
-        <v>4.5657665996798773</v>
+        <v>5.3459621777023081</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
         <v>9.6277999999999989E-2</v>
       </c>
       <c r="J29">
-        <v>1.8741617676773672</v>
+        <v>1.5177064067270183</v>
       </c>
       <c r="K29">
         <v>0.14454722515165275</v>
@@ -1638,7 +1638,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M29">
-        <v>5.1789356222855982</v>
+        <v>5.3459621777023081</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
         <v>0.107678</v>
       </c>
       <c r="J30">
-        <v>1.9224321278524383</v>
+        <v>1.5177064067270183</v>
       </c>
       <c r="K30">
         <v>0.14454722515165275</v>
@@ -1679,7 +1679,7 @@
         <v>4.8441737398371458E-3</v>
       </c>
       <c r="M30">
-        <v>5.4024055380611671</v>
+        <v>5.3459621777023081</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>0.107678</v>
       </c>
       <c r="J31">
-        <v>2.0486053276941791</v>
+        <v>1.5177064067270183</v>
       </c>
       <c r="K31">
         <v>0.14454722515165275</v>
@@ -1720,7 +1720,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M31">
-        <v>5.7921584363662388</v>
+        <v>5.3459621777023081</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>0.37970000000000059</v>
       </c>
       <c r="J32">
-        <v>2.3871156759642926</v>
+        <v>0.73916499635679611</v>
       </c>
       <c r="K32">
         <v>2.4346857984247874E-2</v>
@@ -1761,7 +1761,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M32">
-        <v>3.1819174412533502</v>
+        <v>3.3275967274302025</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>0.40250000000000075</v>
       </c>
       <c r="J33">
-        <v>2.451112047331907</v>
+        <v>0.73916499635679611</v>
       </c>
       <c r="K33">
         <v>2.4346857984247874E-2</v>
@@ -1802,7 +1802,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M33">
-        <v>3.4595790591297884</v>
+        <v>3.3275967274302025</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v>0.39100000000000001</v>
       </c>
       <c r="J34">
-        <v>2.4291279719544843</v>
+        <v>0.73916499635679611</v>
       </c>
       <c r="K34">
         <v>2.4346857984247874E-2</v>
@@ -1843,7 +1843,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M34">
-        <v>3.3607339431546452</v>
+        <v>3.3275967274302025</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1875,7 +1875,7 @@
         <v>0.40240000000000009</v>
       </c>
       <c r="J35">
-        <v>2.4292901038213275</v>
+        <v>0.73916499635679611</v>
       </c>
       <c r="K35">
         <v>2.4346857984247874E-2</v>
@@ -1884,7 +1884,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M35">
-        <v>3.3721453209384951</v>
+        <v>3.3275967274302025</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -1916,7 +1916,7 @@
         <v>0.37970000000000059</v>
       </c>
       <c r="J36">
-        <v>2.4075262283227583</v>
+        <v>0.73916499635679611</v>
       </c>
       <c r="K36">
         <v>2.4346857984247874E-2</v>
@@ -1925,7 +1925,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M36">
-        <v>3.2636078726747333</v>
+        <v>3.3275967274302025</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
         <v>0.37129999999999974</v>
       </c>
       <c r="J37">
-        <v>2.6561593625372391</v>
+        <v>0.91454416270984284</v>
       </c>
       <c r="K37">
         <v>8.9571342534407794E-2</v>
@@ -1966,7 +1966,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M37">
-        <v>4.2282812665219387</v>
+        <v>3.9769952984553631</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>0.32580000000000009</v>
       </c>
       <c r="J38">
-        <v>2.5086724912115059</v>
+        <v>0.91454416270984284</v>
       </c>
       <c r="K38">
         <v>8.9571342534407794E-2</v>
@@ -2007,7 +2007,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M38">
-        <v>3.6019273371692426</v>
+        <v>3.9769952984553631</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
         <v>0.32580000000000009</v>
       </c>
       <c r="J39">
-        <v>2.5086724912115059</v>
+        <v>0.91454416270984284</v>
       </c>
       <c r="K39">
         <v>8.9571342534407794E-2</v>
@@ -2048,7 +2048,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M39">
-        <v>3.6019273371692426</v>
+        <v>3.9769952984553631</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>0.34860000000000024</v>
       </c>
       <c r="J40">
-        <v>2.5965824114396847</v>
+        <v>0.91454416270984284</v>
       </c>
       <c r="K40">
         <v>8.9571342534407794E-2</v>
@@ -2089,7 +2089,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M40">
-        <v>3.9697787490157554</v>
+        <v>3.9769952984553631</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2121,7 +2121,7 @@
         <v>0.40549999999999997</v>
       </c>
       <c r="J41">
-        <v>2.7109811027600665</v>
+        <v>0.91454416270984284</v>
       </c>
       <c r="K41">
         <v>8.9571342534407794E-2</v>
@@ -2130,7 +2130,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M41">
-        <v>4.4830618024006368</v>
+        <v>3.9769952984553631</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
         <v>0.3052999999999999</v>
       </c>
       <c r="J42">
-        <v>2.760164763209862</v>
+        <v>1.118766716801755</v>
       </c>
       <c r="K42">
         <v>5.695230732545685E-2</v>
@@ -2171,7 +2171,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M42">
-        <v>4.5233097176212036</v>
+        <v>4.6922115544403358</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
         <v>0.32809999999999961</v>
       </c>
       <c r="J43">
-        <v>2.8407074886379631</v>
+        <v>1.118766716801755</v>
       </c>
       <c r="K43">
         <v>5.695230732545685E-2</v>
@@ -2212,7 +2212,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M43">
-        <v>4.8611133912594671</v>
+        <v>4.6922115544403358</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>0.33949999999999969</v>
       </c>
       <c r="J44">
-        <v>2.8809788513520145</v>
+        <v>1.118766716801755</v>
       </c>
       <c r="K44">
         <v>5.695230732545685E-2</v>
@@ -2253,7 +2253,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M44">
-        <v>5.0300152280786028</v>
+        <v>4.6922115544403358</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
         <v>0.3052999999999999</v>
       </c>
       <c r="J45">
-        <v>2.760164763209862</v>
+        <v>1.118766716801755</v>
       </c>
       <c r="K45">
         <v>5.695230732545685E-2</v>
@@ -2294,7 +2294,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M45">
-        <v>4.5233097176212036</v>
+        <v>4.6922115544403358</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
         <v>0.3052999999999999</v>
       </c>
       <c r="J46">
-        <v>2.760164763209862</v>
+        <v>1.118766716801755</v>
       </c>
       <c r="K46">
         <v>5.695230732545685E-2</v>
@@ -2335,7 +2335,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M46">
-        <v>4.5233097176212036</v>
+        <v>4.6922115544403358</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>0.30709999999999971</v>
       </c>
       <c r="J47">
-        <v>3.2938539305882522</v>
+        <v>1.4391197709756995</v>
       </c>
       <c r="K47">
         <v>0.10864991079702102</v>
@@ -2376,7 +2376,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M47">
-        <v>6.4564141253770533</v>
+        <v>5.7881844310342121</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>0.29579999999999984</v>
       </c>
       <c r="J48">
-        <v>3.1631673996347049</v>
+        <v>1.4391197709756995</v>
       </c>
       <c r="K48">
         <v>0.10864991079702102</v>
@@ -2417,7 +2417,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M48">
-        <v>5.9660185461186419</v>
+        <v>5.7881844310342121</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>0.27300000000000013</v>
       </c>
       <c r="J49">
-        <v>3.0489748567554429</v>
+        <v>1.4391197709756995</v>
       </c>
       <c r="K49">
         <v>0.10864991079702102</v>
@@ -2458,7 +2458,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M49">
-        <v>5.5061631612251212</v>
+        <v>5.7881844310342121</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2490,7 +2490,7 @@
         <v>0.27300000000000013</v>
       </c>
       <c r="J50">
-        <v>3.0489748567554429</v>
+        <v>1.4391197709756995</v>
       </c>
       <c r="K50">
         <v>0.10864991079702102</v>
@@ -2499,7 +2499,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M50">
-        <v>5.5061631612251212</v>
+        <v>5.7881844310342121</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2531,7 +2531,7 @@
         <v>0.27300000000000013</v>
       </c>
       <c r="J51">
-        <v>3.0489748567554429</v>
+        <v>1.4391197709756995</v>
       </c>
       <c r="K51">
         <v>0.10864991079702102</v>
@@ -2540,7 +2540,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M51">
-        <v>5.5061631612251212</v>
+        <v>5.7881844310342121</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
         <v>0.2407999999999999</v>
       </c>
       <c r="J52">
-        <v>3.7544131321457757</v>
+        <v>2.2106193686255411</v>
       </c>
       <c r="K52">
         <v>0.1165710743311501</v>
@@ -2581,7 +2581,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M52">
-        <v>7.8237013167142848</v>
+        <v>8.2880517623800039</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
         <v>0.22930000000000006</v>
       </c>
       <c r="J53">
-        <v>3.7947478805843109</v>
+        <v>2.2106193686255411</v>
       </c>
       <c r="K53">
         <v>0.1165710743311501</v>
@@ -2622,7 +2622,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M53">
-        <v>7.9099811530488378</v>
+        <v>8.2880517623800039</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
         <v>0.2407999999999999</v>
       </c>
       <c r="J54">
-        <v>3.9007243412114998</v>
+        <v>2.2106193686255411</v>
       </c>
       <c r="K54">
         <v>0.1165710743311501</v>
@@ -2663,7 +2663,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M54">
-        <v>8.3066875780818101</v>
+        <v>8.2880517623800039</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>0.25219999999999998</v>
       </c>
       <c r="J55">
-        <v>4.005779267398454</v>
+        <v>2.2106193686255411</v>
       </c>
       <c r="K55">
         <v>0.1165710743311501</v>
@@ -2704,7 +2704,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M55">
-        <v>8.6999443820275459</v>
+        <v>8.2880517623800039</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -2736,7 +2736,7 @@
         <v>0.25219999999999998</v>
       </c>
       <c r="J56">
-        <v>4.005779267398454</v>
+        <v>2.2106193686255411</v>
       </c>
       <c r="K56">
         <v>0.1165710743311501</v>
@@ -2745,7 +2745,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M56">
-        <v>8.6999443820275459</v>
+        <v>8.2880517623800039</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
         <v>0.21930000000000005</v>
       </c>
       <c r="J57">
-        <v>5.6931722767670312</v>
+        <v>3.6678014392633131</v>
       </c>
       <c r="K57">
         <v>0.21459751257178145</v>
@@ -2786,7 +2786,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M57">
-        <v>13.786530774842291</v>
+        <v>12.714647643742277</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -2818,7 +2818,7 @@
         <v>0.21930000000000005</v>
       </c>
       <c r="J58">
-        <v>5.3591292631456859</v>
+        <v>3.6678014392633131</v>
       </c>
       <c r="K58">
         <v>0.21459751257178145</v>
@@ -2827,7 +2827,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M58">
-        <v>12.778821327762747</v>
+        <v>12.714647643742277</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -2859,7 +2859,7 @@
         <v>0.20789999999999997</v>
       </c>
       <c r="J59">
-        <v>5.1679617194344756</v>
+        <v>3.6678014392633131</v>
       </c>
       <c r="K59">
         <v>0.21459751257178145</v>
@@ -2868,7 +2868,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M59">
-        <v>12.114532394171794</v>
+        <v>12.714647643742277</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>0.20789999999999997</v>
       </c>
       <c r="J60">
-        <v>5.1679617194344756</v>
+        <v>3.6678014392633131</v>
       </c>
       <c r="K60">
         <v>0.21459751257178145</v>
@@ -2909,7 +2909,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M60">
-        <v>12.114532394171794</v>
+        <v>12.714647643742277</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -2941,7 +2941,7 @@
         <v>0.21930000000000005</v>
       </c>
       <c r="J61">
-        <v>5.3591292631456859</v>
+        <v>3.6678014392633131</v>
       </c>
       <c r="K61">
         <v>0.21459751257178145</v>
@@ -2950,7 +2950,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M61">
-        <v>12.778821327762747</v>
+        <v>12.714647643742277</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
         <v>1.1346999999999996</v>
       </c>
       <c r="J62">
-        <v>5.8813300502924157</v>
+        <v>2.2473590884897399</v>
       </c>
       <c r="K62">
         <v>5.0041012236162898E-2</v>
@@ -2991,7 +2991,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M62">
-        <v>9.7530046171293474</v>
+        <v>10.111115925939501</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>1.1802000000000001</v>
       </c>
       <c r="J63">
-        <v>5.9683105224378661</v>
+        <v>2.2473590884897399</v>
       </c>
       <c r="K63">
         <v>5.0041012236162898E-2</v>
@@ -3032,7 +3032,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M63">
-        <v>10.144087467291849</v>
+        <v>10.111115925939501</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>1.2256999999999998</v>
       </c>
       <c r="J64">
-        <v>5.9894042049447282</v>
+        <v>2.2473590884897399</v>
       </c>
       <c r="K64">
         <v>5.0041012236162898E-2</v>
@@ -3073,7 +3073,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M64">
-        <v>10.271467494717474</v>
+        <v>10.111115925939501</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
         <v>1.1688000000000001</v>
       </c>
       <c r="J65">
-        <v>5.9465176129332917</v>
+        <v>2.2473590884897399</v>
       </c>
       <c r="K65">
         <v>5.0041012236162898E-2</v>
@@ -3114,7 +3114,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M65">
-        <v>10.04610187406432</v>
+        <v>10.111115925939501</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -3146,7 +3146,7 @@
         <v>1.2030999999999996</v>
       </c>
       <c r="J66">
-        <v>6.0120875073198601</v>
+        <v>2.2473590884897399</v>
       </c>
       <c r="K66">
         <v>5.0041012236162898E-2</v>
@@ -3155,7 +3155,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M66">
-        <v>10.340918176494508</v>
+        <v>10.111115925939501</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
         <v>0.89759999999999973</v>
       </c>
       <c r="J67">
-        <v>5.9906176881597304</v>
+        <v>2.5325853682033355</v>
       </c>
       <c r="K67">
         <v>0.18203514958543385</v>
@@ -3196,7 +3196,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M67">
-        <v>9.9235419823299864</v>
+        <v>11.038914238917849</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
         <v>1.0911999999999997</v>
       </c>
       <c r="J68">
-        <v>6.4820473894872253</v>
+        <v>2.5325853682033355</v>
       </c>
       <c r="K68">
         <v>0.18203514958543385</v>
@@ -3237,7 +3237,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M68">
-        <v>12.063913782440379</v>
+        <v>11.038914238917849</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
         <v>0.97730000000000006</v>
       </c>
       <c r="J69">
-        <v>6.1929262997082919</v>
+        <v>2.5325853682033355</v>
       </c>
       <c r="K69">
         <v>0.18203514958543385</v>
@@ -3278,7 +3278,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M69">
-        <v>10.804676447561388</v>
+        <v>11.038914238917849</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3310,7 +3310,7 @@
         <v>1.0683999999999996</v>
       </c>
       <c r="J70">
-        <v>6.336579964344784</v>
+        <v>2.5325853682033355</v>
       </c>
       <c r="K70">
         <v>0.18203514958543385</v>
@@ -3319,7 +3319,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M70">
-        <v>11.472833808759917</v>
+        <v>11.038914238917849</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -3351,7 +3351,7 @@
         <v>0.98859999999999992</v>
       </c>
       <c r="J71">
-        <v>6.2216099547961052</v>
+        <v>2.5325853682033355</v>
       </c>
       <c r="K71">
         <v>0.18203514958543385</v>
@@ -3360,7 +3360,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M71">
-        <v>10.929605173497581</v>
+        <v>11.038914238917849</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>0.83079999999999998</v>
       </c>
       <c r="J72">
-        <v>6.5356989347006369</v>
+        <v>2.8104380298463236</v>
       </c>
       <c r="K72">
         <v>5.7899555165353167E-2</v>
@@ -3401,7 +3401,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M72">
-        <v>11.89498949044815</v>
+        <v>11.86069478019566</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3433,7 +3433,7 @@
         <v>0.88770000000000016</v>
       </c>
       <c r="J73">
-        <v>6.6166572536511623</v>
+        <v>2.8104380298463236</v>
       </c>
       <c r="K73">
         <v>5.7899555165353167E-2</v>
@@ -3442,7 +3442,7 @@
         <v>4.0650106703421542E-3</v>
       </c>
       <c r="M73">
-        <v>12.289553333877404</v>
+        <v>11.86069478019566</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>0.81930000000000014</v>
       </c>
       <c r="J74">
-        <v>6.4966154338563253</v>
+        <v>2.8104380298463236</v>
       </c>
       <c r="K74">
         <v>5.7899555165353167E-2</v>
@@ -3483,7 +3483,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M74">
-        <v>11.730338095238531</v>
+        <v>11.86069478019566</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>0.81930000000000014</v>
       </c>
       <c r="J75">
-        <v>6.4966154338563253</v>
+        <v>2.8104380298463236</v>
       </c>
       <c r="K75">
         <v>5.7899555165353167E-2</v>
@@ -3524,7 +3524,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M75">
-        <v>11.730338095238531</v>
+        <v>11.86069478019566</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -3556,7 +3556,7 @@
         <v>0.84209999999999985</v>
       </c>
       <c r="J76">
-        <v>6.4674575486466317</v>
+        <v>2.8104380298463236</v>
       </c>
       <c r="K76">
         <v>5.7899555165353167E-2</v>
@@ -3565,7 +3565,7 @@
         <v>4.0650106703421542E-3</v>
       </c>
       <c r="M76">
-        <v>11.658254886175685</v>
+        <v>11.86069478019566</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -3597,7 +3597,7 @@
         <v>0.6272000000000002</v>
       </c>
       <c r="J77">
-        <v>6.8534675092482598</v>
+        <v>3.2305840446123328</v>
       </c>
       <c r="K77">
         <v>0.12847621977018656</v>
@@ -3606,7 +3606,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M77">
-        <v>12.650056903737712</v>
+        <v>13.036996858863052</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -3638,7 +3638,7 @@
         <v>0.64990000000000014</v>
       </c>
       <c r="J78">
-        <v>6.8207973702289468</v>
+        <v>3.2305840446123328</v>
       </c>
       <c r="K78">
         <v>0.12847621977018656</v>
@@ -3647,7 +3647,7 @@
         <v>4.2481279755395207E-3</v>
       </c>
       <c r="M78">
-        <v>12.586338205665271</v>
+        <v>13.036996858863052</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -3679,7 +3679,7 @@
         <v>0.67280000000000006</v>
       </c>
       <c r="J79">
-        <v>7.0818525950067857</v>
+        <v>3.2305840446123328</v>
       </c>
       <c r="K79">
         <v>0.12847621977018656</v>
@@ -3688,7 +3688,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M79">
-        <v>13.569767673524762</v>
+        <v>13.036996858863052</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
         <v>0.66139999999999999</v>
       </c>
       <c r="J80">
-        <v>6.8758046090503484</v>
+        <v>3.2305840446123328</v>
       </c>
       <c r="K80">
         <v>0.12847621977018656</v>
@@ -3729,7 +3729,7 @@
         <v>4.2481279755395207E-3</v>
       </c>
       <c r="M80">
-        <v>12.809053837862761</v>
+        <v>13.036996858863052</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -3761,7 +3761,7 @@
         <v>0.67279999999999984</v>
       </c>
       <c r="J81">
-        <v>7.0818525950067848</v>
+        <v>3.2305840446123328</v>
       </c>
       <c r="K81">
         <v>0.12847621977018656</v>
@@ -3770,7 +3770,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M81">
-        <v>13.569767673524757</v>
+        <v>13.036996858863052</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -3802,7 +3802,7 @@
         <v>0.49229999999999996</v>
       </c>
       <c r="J82">
-        <v>8.5491504182998312</v>
+        <v>4.9529650601306061</v>
       </c>
       <c r="K82">
         <v>0.20332893637219768</v>
@@ -3811,7 +3811,7 @@
         <v>4.6309623890744174E-3</v>
       </c>
       <c r="M82">
-        <v>17.965174596146092</v>
+        <v>18.423694717077431</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
         <v>0.52639999999999998</v>
       </c>
       <c r="J83">
-        <v>8.8841920633895217</v>
+        <v>4.9529650601306061</v>
       </c>
       <c r="K83">
         <v>0.20332893637219768</v>
@@ -3852,7 +3852,7 @@
         <v>4.6309623890744174E-3</v>
       </c>
       <c r="M83">
-        <v>19.209563086352436</v>
+        <v>18.423694717077431</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -3884,7 +3884,7 @@
         <v>0.52639999999999998</v>
       </c>
       <c r="J84">
-        <v>8.8841920633895217</v>
+        <v>4.9529650601306061</v>
       </c>
       <c r="K84">
         <v>0.20332893637219768</v>
@@ -3893,7 +3893,7 @@
         <v>4.6309623890744174E-3</v>
       </c>
       <c r="M84">
-        <v>19.209563086352436</v>
+        <v>18.423694717077431</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
         <v>0.51509999999999989</v>
       </c>
       <c r="J85">
-        <v>8.4589947927537832</v>
+        <v>4.9529650601306061</v>
       </c>
       <c r="K85">
         <v>0.20332893637219768</v>
@@ -3934,7 +3934,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M85">
-        <v>17.76899822039012</v>
+        <v>18.423694717077431</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -3966,7 +3966,7 @@
         <v>0.49229999999999996</v>
       </c>
       <c r="J86">
-        <v>8.5491504182998312</v>
+        <v>4.9529650601306061</v>
       </c>
       <c r="K86">
         <v>0.20332893637219768</v>
@@ -3975,7 +3975,7 @@
         <v>4.6309623890744174E-3</v>
       </c>
       <c r="M86">
-        <v>17.965174596146092</v>
+        <v>18.423694717077431</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -4007,7 +4007,7 @@
         <v>0.41332000000000002</v>
       </c>
       <c r="J87">
-        <v>10.036821086372093</v>
+        <v>6.4990937552930124</v>
       </c>
       <c r="K87">
         <v>0.24670044844442024</v>
@@ -4016,7 +4016,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M87">
-        <v>22.233092413667542</v>
+        <v>22.846315227748182</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4048,7 +4048,7 @@
         <v>0.44752000000000003</v>
       </c>
       <c r="J88">
-        <v>10.560151766422528</v>
+        <v>6.4990937552930124</v>
       </c>
       <c r="K88">
         <v>0.24670044844442024</v>
@@ -4057,7 +4057,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M88">
-        <v>24.072760855909461</v>
+        <v>22.846315227748182</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4089,7 +4089,7 @@
         <v>0.43611999999999995</v>
       </c>
       <c r="J89">
-        <v>10.385708206405715</v>
+        <v>6.4990937552930124</v>
       </c>
       <c r="K89">
         <v>0.24670044844442024</v>
@@ -4098,7 +4098,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M89">
-        <v>23.459538041828818</v>
+        <v>22.846315227748182</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -4130,7 +4130,7 @@
         <v>0.41332000000000002</v>
       </c>
       <c r="J90">
-        <v>10.036821086372093</v>
+        <v>6.4990937552930124</v>
       </c>
       <c r="K90">
         <v>0.24670044844442024</v>
@@ -4139,7 +4139,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M90">
-        <v>22.233092413667542</v>
+        <v>22.846315227748182</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4171,7 +4171,7 @@
         <v>0.41332000000000002</v>
       </c>
       <c r="J91">
-        <v>10.036821086372093</v>
+        <v>6.4990937552930124</v>
       </c>
       <c r="K91">
         <v>0.24670044844442024</v>
@@ -4180,7 +4180,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M91">
-        <v>22.233092413667542</v>
+        <v>22.846315227748182</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>0.60959999999999948</v>
       </c>
       <c r="J92">
-        <v>3.4630621286971968</v>
+        <v>1.1418522768985848</v>
       </c>
       <c r="K92">
         <v>6.4339605623299337E-2</v>
@@ -4221,7 +4221,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M92">
-        <v>5.2396506694298477</v>
+        <v>5.130472254206099</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>0.62099999999999955</v>
       </c>
       <c r="J93">
-        <v>3.5197398189729743</v>
+        <v>1.1418522768985848</v>
       </c>
       <c r="K93">
         <v>6.4339605623299337E-2</v>
@@ -4262,7 +4262,7 @@
         <v>3.8378048403035683E-3</v>
       </c>
       <c r="M93">
-        <v>5.4767838163837084</v>
+        <v>5.130472254206099</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>0.55269999999999975</v>
       </c>
       <c r="J94">
-        <v>3.3542887470471729</v>
+        <v>1.1418522768985848</v>
       </c>
       <c r="K94">
         <v>6.4339605623299337E-2</v>
@@ -4303,7 +4303,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M94">
-        <v>4.7505822260398256</v>
+        <v>5.130472254206099</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -4335,7 +4335,7 @@
         <v>0.60959999999999948</v>
       </c>
       <c r="J95">
-        <v>3.4630621286971968</v>
+        <v>1.1418522768985848</v>
       </c>
       <c r="K95">
         <v>6.4339605623299337E-2</v>
@@ -4344,7 +4344,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M95">
-        <v>5.2396506694298477</v>
+        <v>5.130472254206099</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4376,7 +4376,7 @@
         <v>0.57539999999999925</v>
       </c>
       <c r="J96">
-        <v>3.3976834001834737</v>
+        <v>1.1418522768985848</v>
       </c>
       <c r="K96">
         <v>6.4339605623299337E-2</v>
@@ -4385,7 +4385,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M96">
-        <v>4.9456938897472646</v>
+        <v>5.130472254206099</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -4417,7 +4417,7 @@
         <v>0.49840000000000018</v>
       </c>
       <c r="J97">
-        <v>3.6057833566765987</v>
+        <v>1.3321091321178535</v>
       </c>
       <c r="K97">
         <v>4.917926752651719E-2</v>
@@ -4426,7 +4426,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M97">
-        <v>5.6756676090345719</v>
+        <v>5.779979638125174</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4458,7 +4458,7 @@
         <v>0.53259999999999996</v>
       </c>
       <c r="J98">
-        <v>3.6955424636165279</v>
+        <v>1.3321091321178535</v>
       </c>
       <c r="K98">
         <v>4.917926752651719E-2</v>
@@ -4467,7 +4467,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M98">
-        <v>6.0651295517090933</v>
+        <v>5.779979638125174</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4499,7 +4499,7 @@
         <v>0.49849999999999994</v>
       </c>
       <c r="J99">
-        <v>3.6060458102056625</v>
+        <v>1.3321091321178535</v>
       </c>
       <c r="K99">
         <v>4.917926752651719E-2</v>
@@ -4508,7 +4508,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M99">
-        <v>5.6768063866447296</v>
+        <v>5.779979638125174</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4540,7 +4540,7 @@
         <v>0.5213000000000001</v>
       </c>
       <c r="J100">
-        <v>3.665885214832282</v>
+        <v>1.3321091321178535</v>
       </c>
       <c r="K100">
         <v>4.917926752651719E-2</v>
@@ -4549,7 +4549,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M100">
-        <v>5.936447681761079</v>
+        <v>5.779979638125174</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>0.48699999999999966</v>
       </c>
       <c r="J101">
-        <v>3.5758636543632871</v>
+        <v>1.3321091321178535</v>
       </c>
       <c r="K101">
         <v>4.917926752651719E-2</v>
@@ -4590,7 +4590,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M101">
-        <v>5.545846961476391</v>
+        <v>5.779979638125174</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4622,7 +4622,7 @@
         <v>0.46580000000000021</v>
       </c>
       <c r="J102">
-        <v>3.8807666802802028</v>
+        <v>1.6126149032096155</v>
       </c>
       <c r="K102">
         <v>4.6724555845190197E-2</v>
@@ -4631,7 +4631,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M102">
-        <v>6.6690973816210297</v>
+        <v>6.7751642590115591</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4663,7 +4663,7 @@
         <v>0.45439999999999969</v>
       </c>
       <c r="J103">
-        <v>3.8420230359649699</v>
+        <v>1.6126149032096155</v>
       </c>
       <c r="K103">
         <v>4.6724555845190197E-2</v>
@@ -4672,7 +4672,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M103">
-        <v>6.5058777376740924</v>
+        <v>6.7751642590115591</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4704,7 +4704,7 @@
         <v>0.4657</v>
       </c>
       <c r="J104">
-        <v>3.9428354604467764</v>
+        <v>1.6126149032096155</v>
       </c>
       <c r="K104">
         <v>4.6724555845190197E-2</v>
@@ -4713,7 +4713,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M104">
-        <v>6.8997881935676206</v>
+        <v>6.7751642590115591</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4745,7 +4745,7 @@
         <v>0.4657</v>
       </c>
       <c r="J105">
-        <v>3.9428354604467764</v>
+        <v>1.6126149032096155</v>
       </c>
       <c r="K105">
         <v>4.6724555845190197E-2</v>
@@ -4754,7 +4754,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M105">
-        <v>6.8997881935676206</v>
+        <v>6.7751642590115591</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4786,7 +4786,7 @@
         <v>0.46579999999999977</v>
       </c>
       <c r="J106">
-        <v>3.9431887180144427</v>
+        <v>1.6126149032096155</v>
       </c>
       <c r="K106">
         <v>4.6724555845190197E-2</v>
@@ -4795,7 +4795,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M106">
-        <v>6.9012697886274346</v>
+        <v>6.7751642590115591</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4827,7 +4827,7 @@
         <v>0.36509999999999998</v>
       </c>
       <c r="J107">
-        <v>4.3188411706634042</v>
+        <v>2.1474535102892869</v>
       </c>
       <c r="K107">
         <v>7.7291957828899319E-2</v>
@@ -4836,7 +4836,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M107">
-        <v>8.0435382284178889</v>
+        <v>8.5462869065129219</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -4868,7 +4868,7 @@
         <v>0.39929999999999999</v>
       </c>
       <c r="J108">
-        <v>4.5081660573717297</v>
+        <v>2.1474535102892869</v>
       </c>
       <c r="K108">
         <v>7.7291957828899319E-2</v>
@@ -4877,7 +4877,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M108">
-        <v>8.7970003139064996</v>
+        <v>8.5462869065129219</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4909,7 +4909,7 @@
         <v>0.39929999999999999</v>
       </c>
       <c r="J109">
-        <v>4.5081660573717297</v>
+        <v>2.1474535102892869</v>
       </c>
       <c r="K109">
         <v>7.7291957828899319E-2</v>
@@ -4918,7 +4918,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M109">
-        <v>8.7970003139064996</v>
+        <v>8.5462869065129219</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -4950,7 +4950,7 @@
         <v>0.38789999999999991</v>
       </c>
       <c r="J110">
-        <v>4.4450577618022873</v>
+        <v>2.1474535102892869</v>
       </c>
       <c r="K110">
         <v>7.7291957828899319E-2</v>
@@ -4959,7 +4959,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M110">
-        <v>8.5458462854102937</v>
+        <v>8.5462869065129219</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
         <v>0.38800000000000012</v>
       </c>
       <c r="J111">
-        <v>4.4456113433423718</v>
+        <v>2.1474535102892869</v>
       </c>
       <c r="K111">
         <v>7.7291957828899319E-2</v>
@@ -5000,7 +5000,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M111">
-        <v>8.5480493909234241</v>
+        <v>8.5462869065129219</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -5032,7 +5032,7 @@
         <v>0.35489999999999999</v>
       </c>
       <c r="J112">
-        <v>5.174406490463543</v>
+        <v>2.8212489472272688</v>
       </c>
       <c r="K112">
         <v>5.0611915335195844E-2</v>
@@ -5041,7 +5041,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M112">
-        <v>10.937693302431672</v>
+        <v>10.726890760339163</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5073,7 +5073,7 @@
         <v>0.34350000000000014</v>
       </c>
       <c r="J113">
-        <v>5.0820021981047816</v>
+        <v>2.8212489472272688</v>
       </c>
       <c r="K113">
         <v>5.0611915335195844E-2</v>
@@ -5082,7 +5082,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M113">
-        <v>10.586355732277489</v>
+        <v>10.726890760339163</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5114,7 +5114,7 @@
         <v>0.35489999999999999</v>
       </c>
       <c r="J114">
-        <v>5.174406490463543</v>
+        <v>2.8212489472272688</v>
       </c>
       <c r="K114">
         <v>5.0611915335195844E-2</v>
@@ -5123,7 +5123,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M114">
-        <v>10.937693302431672</v>
+        <v>10.726890760339163</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -5155,7 +5155,7 @@
         <v>0.34350000000000014</v>
       </c>
       <c r="J115">
-        <v>5.0820021981047816</v>
+        <v>2.8212489472272688</v>
       </c>
       <c r="K115">
         <v>5.0611915335195844E-2</v>
@@ -5164,7 +5164,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M115">
-        <v>10.586355732277489</v>
+        <v>10.726890760339163</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>0.34350000000000014</v>
       </c>
       <c r="J116">
-        <v>5.0820021981047816</v>
+        <v>2.8212489472272688</v>
       </c>
       <c r="K116">
         <v>5.0611915335195844E-2</v>
@@ -5205,7 +5205,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M116">
-        <v>10.586355732277489</v>
+        <v>10.726890760339163</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -5237,7 +5237,7 @@
         <v>0.28781999999999985</v>
       </c>
       <c r="J117">
-        <v>7.1241923740456015</v>
+        <v>4.7310110371834995</v>
       </c>
       <c r="K117">
         <v>0.23946352647817809</v>
@@ -5246,7 +5246,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M117">
-        <v>16.77154744439887</v>
+        <v>16.512411570187453</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -5278,7 +5278,7 @@
         <v>0.29921999999999993</v>
       </c>
       <c r="J118">
-        <v>6.8763993562622838</v>
+        <v>4.7310110371834995</v>
       </c>
       <c r="K118">
         <v>0.23946352647817809</v>
@@ -5287,7 +5287,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M118">
-        <v>16.095485125369205</v>
+        <v>16.512411570187453</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -5319,7 +5319,7 @@
         <v>0.28792000000000006</v>
       </c>
       <c r="J119">
-        <v>6.703486002912288</v>
+        <v>4.7310110371834995</v>
       </c>
       <c r="K119">
         <v>0.23946352647817809</v>
@@ -5328,7 +5328,7 @@
         <v>4.8928858538759513E-3</v>
       </c>
       <c r="M119">
-        <v>15.487641458780509</v>
+        <v>16.512411570187453</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -5360,7 +5360,7 @@
         <v>0.28781999999999996</v>
       </c>
       <c r="J120">
-        <v>7.1241923740456032</v>
+        <v>4.7310110371834995</v>
       </c>
       <c r="K120">
         <v>0.23946352647817809</v>
@@ -5369,7 +5369,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M120">
-        <v>16.771547444398873</v>
+        <v>16.512411570187453</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5401,7 +5401,7 @@
         <v>0.29921999999999993</v>
       </c>
       <c r="J121">
-        <v>7.3153599177568118</v>
+        <v>4.7310110371834995</v>
       </c>
       <c r="K121">
         <v>0.23946352647817809</v>
@@ -5410,7 +5410,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M121">
-        <v>17.435836377989823</v>
+        <v>16.512411570187453</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -5442,7 +5442,7 @@
         <v>-0.11280000000000001</v>
       </c>
       <c r="J122">
-        <v>0.46292213111109981</v>
+        <v>-0.21055244023096059</v>
       </c>
       <c r="K122">
         <v>1.3064432842557049E-2</v>
@@ -5451,7 +5451,7 @@
         <v>3.8378048403035683E-3</v>
       </c>
       <c r="M122">
-        <v>-0.99481677051221062</v>
+        <v>-0.94482522287827631</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -5483,7 +5483,7 @@
         <v>-0.10139999999999993</v>
       </c>
       <c r="J123">
-        <v>0.48535543755736776</v>
+        <v>-0.21055244023096059</v>
       </c>
       <c r="K123">
         <v>1.3064432842557049E-2</v>
@@ -5492,7 +5492,7 @@
         <v>3.8378048403035683E-3</v>
       </c>
       <c r="M123">
-        <v>-0.89427677774767789</v>
+        <v>-0.94482522287827631</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -5524,7 +5524,7 @@
         <v>-0.11280000000000023</v>
       </c>
       <c r="J124">
-        <v>0.46925869032364642</v>
+        <v>-0.21055244023096059</v>
       </c>
       <c r="K124">
         <v>1.3064432842557049E-2</v>
@@ -5533,7 +5533,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M124">
-        <v>-0.96954165930395086</v>
+        <v>-0.94482522287827631</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -5565,7 +5565,7 @@
         <v>-0.11270000000000002</v>
       </c>
       <c r="J125">
-        <v>0.46311891450097931</v>
+        <v>-0.21055244023096059</v>
       </c>
       <c r="K125">
         <v>1.3064432842557049E-2</v>
@@ -5574,7 +5574,7 @@
         <v>3.8378048403035683E-3</v>
       </c>
       <c r="M125">
-        <v>-0.99393484075111838</v>
+        <v>-0.94482522287827631</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -5606,7 +5606,7 @@
         <v>-0.10140000000000016</v>
       </c>
       <c r="J126">
-        <v>0.49105159982822078</v>
+        <v>-0.21055244023096059</v>
       </c>
       <c r="K126">
         <v>1.3064432842557049E-2</v>
@@ -5615,7 +5615,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M126">
-        <v>-0.87155606607642344</v>
+        <v>-0.94482522287827631</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -5647,7 +5647,7 @@
         <v>-4.3500000000000094E-2</v>
       </c>
       <c r="J127">
-        <v>0.57804074857705878</v>
+        <v>-0.11421662410471001</v>
       </c>
       <c r="K127">
         <v>4.6996061352230258E-2</v>
@@ -5656,7 +5656,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M127">
-        <v>-0.46711743792686039</v>
+        <v>-0.49909529216989423</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -5688,7 +5688,7 @@
         <v>-5.4899999999999949E-2</v>
       </c>
       <c r="J128">
-        <v>0.55003788126609199</v>
+        <v>-0.11421662410471001</v>
       </c>
       <c r="K128">
         <v>4.6996061352230258E-2</v>
@@ -5697,7 +5697,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M128">
-        <v>-0.58953442165941505</v>
+        <v>-0.49909529216989423</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5729,7 +5729,7 @@
         <v>-2.0699999999999941E-2</v>
       </c>
       <c r="J129">
-        <v>0.6323494001768396</v>
+        <v>-0.11421662410471001</v>
       </c>
       <c r="K129">
         <v>4.6996061352230258E-2</v>
@@ -5738,7 +5738,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M129">
-        <v>-0.22885173689196772</v>
+        <v>-0.49909529216989423</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -5770,7 +5770,7 @@
         <v>-6.6199999999999815E-2</v>
       </c>
       <c r="J130">
-        <v>0.52228065314206329</v>
+        <v>-0.11421662410471001</v>
       </c>
       <c r="K130">
         <v>4.6996061352230258E-2</v>
@@ -5779,7 +5779,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M130">
-        <v>-0.71087757220133352</v>
+        <v>-0.49909529216989423</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -5811,7 +5811,7 @@
         <v>3.7449999999999983E-2</v>
       </c>
       <c r="J131">
-        <v>0.81718875398655821</v>
+        <v>0.13440235973131903</v>
       </c>
       <c r="K131">
         <v>2.976657795448891E-2</v>
@@ -5820,7 +5820,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M131">
-        <v>0.55485734990145441</v>
+        <v>0.56264767198803411</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -5852,7 +5852,7 @@
         <v>3.7420000000000009E-2</v>
       </c>
       <c r="J132">
-        <v>0.81708277671625817</v>
+        <v>0.13440235973131903</v>
       </c>
       <c r="K132">
         <v>2.976657795448891E-2</v>
@@ -5861,7 +5861,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M132">
-        <v>0.5544128713835097</v>
+        <v>0.56264767198803411</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -5893,7 +5893,7 @@
         <v>4.885000000000006E-2</v>
       </c>
       <c r="J133">
-        <v>0.86440149982437853</v>
+        <v>0.13440235973131903</v>
       </c>
       <c r="K133">
         <v>2.976657795448891E-2</v>
@@ -5902,7 +5902,7 @@
         <v>4.1197123055157318E-3</v>
       </c>
       <c r="M133">
-        <v>0.74945343165047806</v>
+        <v>0.56264767198803411</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5934,7 +5934,7 @@
         <v>3.7449999999999983E-2</v>
       </c>
       <c r="J134">
-        <v>0.81718875398655821</v>
+        <v>0.13440235973131903</v>
       </c>
       <c r="K134">
         <v>2.976657795448891E-2</v>
@@ -5943,7 +5943,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M134">
-        <v>0.55485734990145441</v>
+        <v>0.56264767198803411</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5975,7 +5975,7 @@
         <v>2.6050000000000018E-2</v>
       </c>
       <c r="J135">
-        <v>0.78061898861895906</v>
+        <v>0.13440235973131903</v>
       </c>
       <c r="K135">
         <v>2.976657795448891E-2</v>
@@ -5984,7 +5984,7 @@
         <v>4.1197123055157318E-3</v>
       </c>
       <c r="M135">
-        <v>0.39965735710327416</v>
+        <v>0.56264767198803411</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -6016,7 +6016,7 @@
         <v>7.2429999999999994E-2</v>
       </c>
       <c r="J136">
-        <v>1.0476554563314093</v>
+        <v>0.38212882224311373</v>
       </c>
       <c r="K136">
         <v>3.485111662056873E-2</v>
@@ -6025,7 +6025,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M136">
-        <v>1.4608476108700925</v>
+        <v>1.5403511090266608</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -6057,7 +6057,7 @@
         <v>7.2350000000000025E-2</v>
       </c>
       <c r="J137">
-        <v>1.0472547807423596</v>
+        <v>0.38212882224311373</v>
       </c>
       <c r="K137">
         <v>3.485111662056873E-2</v>
@@ -6066,7 +6066,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M137">
-        <v>1.4592340832038</v>
+        <v>1.5403511090266608</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -6098,7 +6098,7 @@
         <v>8.3780000000000077E-2</v>
       </c>
       <c r="J138">
-        <v>1.1045013055278852</v>
+        <v>0.38212882224311373</v>
       </c>
       <c r="K138">
         <v>3.485111662056873E-2</v>
@@ -6107,7 +6107,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M138">
-        <v>1.6897668485254242</v>
+        <v>1.5403511090266608</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -6139,7 +6139,7 @@
         <v>7.240000000000002E-2</v>
       </c>
       <c r="J139">
-        <v>1.0312002375621461</v>
+        <v>0.38212882224311373</v>
       </c>
       <c r="K139">
         <v>3.485111662056873E-2</v>
@@ -6148,7 +6148,7 @@
         <v>4.2481279755395207E-3</v>
       </c>
       <c r="M139">
-        <v>1.4021401540085638</v>
+        <v>1.5403511090266608</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -6180,7 +6180,7 @@
         <v>8.3780000000000077E-2</v>
       </c>
       <c r="J140">
-        <v>1.1045013055278852</v>
+        <v>0.38212882224311373</v>
       </c>
       <c r="K140">
         <v>3.485111662056873E-2</v>
@@ -6189,7 +6189,7 @@
         <v>4.271150892313883E-3</v>
       </c>
       <c r="M140">
-        <v>1.6897668485254242</v>
+        <v>1.5403511090266608</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -6221,7 +6221,7 @@
         <v>0.130329</v>
       </c>
       <c r="J141">
-        <v>1.8067319040229026</v>
+        <v>1.1338182963874843</v>
       </c>
       <c r="K141">
         <v>7.3239562799725655E-2</v>
@@ -6230,7 +6230,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M141">
-        <v>4.2344483758557159</v>
+        <v>4.2646720086035685</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -6262,7 +6262,7 @@
         <v>0.11891</v>
       </c>
       <c r="J142">
-        <v>1.7084401242338383</v>
+        <v>1.1338182963874843</v>
       </c>
       <c r="K142">
         <v>7.3239562799725655E-2</v>
@@ -6271,7 +6271,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M142">
-        <v>3.8634398819372753</v>
+        <v>4.2646720086035685</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -6303,7 +6303,7 @@
         <v>0.13030900000000001</v>
       </c>
       <c r="J143">
-        <v>1.8857361086229236</v>
+        <v>1.1338182963874843</v>
       </c>
       <c r="K143">
         <v>7.3239562799725655E-2</v>
@@ -6312,7 +6312,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M143">
-        <v>4.4951667425758428</v>
+        <v>4.2646720086035685</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -6344,7 +6344,7 @@
         <v>0.130329</v>
       </c>
       <c r="J144">
-        <v>1.8067319040229026</v>
+        <v>1.1338182963874843</v>
       </c>
       <c r="K144">
         <v>7.3239562799725655E-2</v>
@@ -6353,7 +6353,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M144">
-        <v>4.2344483758557159</v>
+        <v>4.2646720086035685</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -6385,7 +6385,7 @@
         <v>0.130329</v>
       </c>
       <c r="J145">
-        <v>1.8859204155109708</v>
+        <v>1.1338182963874843</v>
       </c>
       <c r="K145">
         <v>7.3239562799725655E-2</v>
@@ -6394,7 +6394,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M145">
-        <v>4.4958566667932915</v>
+        <v>4.2646720086035685</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -6426,7 +6426,7 @@
         <v>0.15368899999999999</v>
       </c>
       <c r="J146">
-        <v>3.2621173585296139</v>
+        <v>2.6239602715451071</v>
       </c>
       <c r="K146">
         <v>0.17088918637464251</v>
@@ -6435,7 +6435,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M146">
-        <v>8.9556054311104809</v>
+        <v>9.0965579041419584</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -6467,7 +6467,7 @@
         <v>0.142289</v>
       </c>
       <c r="J147">
-        <v>3.0709498148184053</v>
+        <v>2.6239602715451071</v>
       </c>
       <c r="K147">
         <v>0.17088918637464251</v>
@@ -6476,7 +6476,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M147">
-        <v>8.2913164975195333</v>
+        <v>9.0965579041419584</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -6508,7 +6508,7 @@
         <v>0.15368899999999999</v>
       </c>
       <c r="J148">
-        <v>3.2621173585296139</v>
+        <v>2.6239602715451071</v>
       </c>
       <c r="K148">
         <v>0.17088918637464251</v>
@@ -6517,7 +6517,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M148">
-        <v>8.9556054311104809</v>
+        <v>9.0965579041419584</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -6549,7 +6549,7 @@
         <v>0.16506399999999999</v>
       </c>
       <c r="J149">
-        <v>3.4528656751712816</v>
+        <v>2.6239602715451071</v>
       </c>
       <c r="K149">
         <v>0.17088918637464251</v>
@@ -6558,7 +6558,7 @@
         <v>4.949776498696737E-3</v>
       </c>
       <c r="M149">
-        <v>9.618437590724259</v>
+        <v>9.0965579041419584</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -6590,7 +6590,7 @@
         <v>0.15368899999999999</v>
       </c>
       <c r="J150">
-        <v>3.4962201251527372</v>
+        <v>2.6239602715451071</v>
       </c>
       <c r="K150">
         <v>0.17088918637464251</v>
@@ -6599,7 +6599,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M150">
-        <v>9.6618245702450363</v>
+        <v>9.0965579041419584</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -6631,7 +6631,7 @@
         <v>-2.7944</v>
       </c>
       <c r="J151">
-        <v>-9.8350722340230838</v>
+        <v>-5.1930750094257743</v>
       </c>
       <c r="K151">
         <v>0.24900210507797238</v>
@@ -6640,7 +6640,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M151">
-        <v>-24.018503659210587</v>
+        <v>-23.377644076675537</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -6672,7 +6672,7 @@
         <v>-2.8742999999999994</v>
       </c>
       <c r="J152">
-        <v>-9.9878137664279514</v>
+        <v>-5.1930750094257743</v>
       </c>
       <c r="K152">
         <v>0.24900210507797238</v>
@@ -6681,7 +6681,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M152">
-        <v>-24.705262334550881</v>
+        <v>-23.377644076675537</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -6713,7 +6713,7 @@
         <v>-2.6009999999999995</v>
       </c>
       <c r="J153">
-        <v>-9.3255421957882518</v>
+        <v>-5.1930750094257743</v>
       </c>
       <c r="K153">
         <v>0.24900210507797238</v>
@@ -6722,7 +6722,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M153">
-        <v>-21.796595377139713</v>
+        <v>-23.377644076675537</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -6754,7 +6754,7 @@
         <v>-2.7033000000000005</v>
       </c>
       <c r="J154">
-        <v>-9.6609201238593378</v>
+        <v>-5.1930750094257743</v>
       </c>
       <c r="K154">
         <v>0.24900210507797238</v>
@@ -6763,7 +6763,7 @@
         <v>3.8254403645675409E-3</v>
       </c>
       <c r="M154">
-        <v>-23.235478436137985</v>
+        <v>-23.377644076675537</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -6795,7 +6795,7 @@
         <v>-2.7604000000000002</v>
       </c>
       <c r="J155">
-        <v>-9.6216921429429458</v>
+        <v>-5.1930750094257743</v>
       </c>
       <c r="K155">
         <v>0.24900210507797238</v>
@@ -6804,7 +6804,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M155">
-        <v>-23.132380576338523</v>
+        <v>-23.377644076675537</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -6836,7 +6836,7 @@
         <v>-2.0522</v>
       </c>
       <c r="J156">
-        <v>-9.7023894523162415</v>
+        <v>-5.1240782228040853</v>
       </c>
       <c r="K156">
         <v>0.2729539863679224</v>
@@ -6845,7 +6845,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M156">
-        <v>-22.688383306748673</v>
+        <v>-22.333449908797508</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -6877,7 +6877,7 @@
         <v>-2.0181000000000004</v>
       </c>
       <c r="J157">
-        <v>-9.4503775147845541</v>
+        <v>-5.1240782228040853</v>
       </c>
       <c r="K157">
         <v>0.2729539863679224</v>
@@ -6886,7 +6886,7 @@
         <v>3.9344975105814802E-3</v>
       </c>
       <c r="M157">
-        <v>-21.671027620234373</v>
+        <v>-22.333449908797508</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -6918,7 +6918,7 @@
         <v>-1.9838</v>
       </c>
       <c r="J158">
-        <v>-9.5287644958554942</v>
+        <v>-5.1240782228040853</v>
       </c>
       <c r="K158">
         <v>0.2729539863679224</v>
@@ -6927,7 +6927,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M158">
-        <v>-21.932177567453468</v>
+        <v>-22.333449908797508</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -6959,7 +6959,7 @@
         <v>-2.1888000000000005</v>
       </c>
       <c r="J159">
-        <v>-10.049131689926448</v>
+        <v>-5.1240782228040853</v>
       </c>
       <c r="K159">
         <v>0.2729539863679224</v>
@@ -6968,7 +6968,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M159">
-        <v>-24.198583657446399</v>
+        <v>-22.333449908797508</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -7000,7 +7000,7 @@
         <v>-1.9155000000000006</v>
       </c>
       <c r="J160">
-        <v>-9.3553933770503939</v>
+        <v>-5.1240782228040853</v>
       </c>
       <c r="K160">
         <v>0.2729539863679224</v>
@@ -7009,7 +7009,7 @@
         <v>3.9491227002696281E-3</v>
       </c>
       <c r="M160">
-        <v>-21.177077392104618</v>
+        <v>-22.333449908797508</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -7041,7 +7041,7 @@
         <v>-1.4120000000000001</v>
       </c>
       <c r="J161">
-        <v>-9.4811299386422156</v>
+        <v>-4.7627222986341007</v>
       </c>
       <c r="K161">
         <v>0.29152295040785703</v>
@@ -7050,7 +7050,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M161">
-        <v>-20.920122244615595</v>
+        <v>-20.009928760795013</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -7082,7 +7082,7 @@
         <v>-1.2984</v>
       </c>
       <c r="J162">
-        <v>-9.0798293417723723</v>
+        <v>-4.7627222986341007</v>
       </c>
       <c r="K162">
         <v>0.29152295040785703</v>
@@ -7091,7 +7091,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M162">
-        <v>-19.23703025666352</v>
+        <v>-20.009928760795013</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -7123,7 +7123,7 @@
         <v>-1.4121999999999999</v>
       </c>
       <c r="J163">
-        <v>-9.4818364537775484</v>
+        <v>-4.7627222986341007</v>
       </c>
       <c r="K163">
         <v>0.29152295040785703</v>
@@ -7132,7 +7132,7 @@
         <v>4.1010059554498013E-3</v>
       </c>
       <c r="M163">
-        <v>-20.923085434735221</v>
+        <v>-20.009928760795013</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -7164,7 +7164,7 @@
         <v>-1.4464999999999999</v>
       </c>
       <c r="J164">
-        <v>-9.4091577763388514</v>
+        <v>-4.7627222986341007</v>
       </c>
       <c r="K164">
         <v>0.29152295040785703</v>
@@ -7173,7 +7173,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M164">
-        <v>-20.710282014845031</v>
+        <v>-20.009928760795013</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -7205,7 +7205,7 @@
         <v>-1.2752999999999999</v>
       </c>
       <c r="J165">
-        <v>-8.8273233985522204</v>
+        <v>-4.7627222986341007</v>
       </c>
       <c r="K165">
         <v>0.29152295040785703</v>
@@ -7214,7 +7214,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M165">
-        <v>-18.2591238531157</v>
+        <v>-20.009928760795013</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -7246,7 +7246,7 @@
         <v>-0.82910000000000017</v>
       </c>
       <c r="J166">
-        <v>-9.0828776320092253</v>
+        <v>-4.9220032633396276</v>
       </c>
       <c r="K166">
         <v>0.28888273330833097</v>
@@ -7255,7 +7255,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M166">
-        <v>-18.265947809316003</v>
+        <v>-19.495060428132952</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -7287,7 +7287,7 @@
         <v>-0.84060000000000001</v>
       </c>
       <c r="J167">
-        <v>-9.3826380464939803</v>
+        <v>-4.9220032633396276</v>
       </c>
       <c r="K167">
         <v>0.28888273330833097</v>
@@ -7296,7 +7296,7 @@
         <v>4.3473233346519764E-3</v>
       </c>
       <c r="M167">
-        <v>-19.34511856953684</v>
+        <v>-19.495060428132952</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -7328,7 +7328,7 @@
         <v>-0.92017000000000004</v>
       </c>
       <c r="J168">
-        <v>-9.8454716295664184</v>
+        <v>-4.9220032633396276</v>
       </c>
       <c r="K168">
         <v>0.28888273330833097</v>
@@ -7337,7 +7337,7 @@
         <v>4.3473233346519764E-3</v>
       </c>
       <c r="M168">
-        <v>-21.176299969225209</v>
+        <v>-19.495060428132952</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -7369,7 +7369,7 @@
         <v>-0.86330000000000018</v>
       </c>
       <c r="J169">
-        <v>-9.5146767839043651</v>
+        <v>-4.9220032633396276</v>
       </c>
       <c r="K169">
         <v>0.28888273330833097</v>
@@ -7378,7 +7378,7 @@
         <v>4.3473233346519764E-3</v>
       </c>
       <c r="M169">
-        <v>-19.867524222080839</v>
+        <v>-19.495060428132952</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -7410,7 +7410,7 @@
         <v>-0.81780000000000008</v>
       </c>
       <c r="J170">
-        <v>-9.2500176406368535</v>
+        <v>-4.9220032633396276</v>
       </c>
       <c r="K170">
         <v>0.28888273330833097</v>
@@ -7419,7 +7419,7 @@
         <v>4.3473233346519764E-3</v>
       </c>
       <c r="M170">
-        <v>-18.820411570505861</v>
+        <v>-19.495060428132952</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -7451,7 +7451,7 @@
         <v>-0.46373000000000009</v>
       </c>
       <c r="J171">
-        <v>-8.484800220548582</v>
+        <v>-4.3091230759176486</v>
       </c>
       <c r="K171">
         <v>0.36213927762322257</v>
@@ -7460,7 +7460,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M171">
-        <v>-15.066798220929888</v>
+        <v>-16.434185094589779</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -7492,7 +7492,7 @@
         <v>-0.53207999999999989</v>
       </c>
       <c r="J172">
-        <v>-8.5617545881628381</v>
+        <v>-4.3091230759176486</v>
       </c>
       <c r="K172">
         <v>0.36213927762322257</v>
@@ -7501,7 +7501,7 @@
         <v>4.491965225630939E-3</v>
       </c>
       <c r="M172">
-        <v>-15.578991904558155</v>
+        <v>-16.434185094589779</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -7533,7 +7533,7 @@
         <v>-0.63458000000000014</v>
       </c>
       <c r="J173">
-        <v>-9.345534666836123</v>
+        <v>-4.3091230759176486</v>
       </c>
       <c r="K173">
         <v>0.36213927762322257</v>
@@ -7542,7 +7542,7 @@
         <v>4.491965225630939E-3</v>
       </c>
       <c r="M173">
-        <v>-18.580132090652754</v>
+        <v>-16.434185094589779</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -7574,7 +7574,7 @@
         <v>-0.58908000000000005</v>
       </c>
       <c r="J174">
-        <v>-8.9976127782543251</v>
+        <v>-4.3091230759176486</v>
       </c>
       <c r="K174">
         <v>0.36213927762322257</v>
@@ -7583,7 +7583,7 @@
         <v>4.491965225630939E-3</v>
       </c>
       <c r="M174">
-        <v>-17.247918642191248</v>
+        <v>-16.434185094589779</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -7615,7 +7615,7 @@
         <v>-0.50932999999999995</v>
       </c>
       <c r="J175">
-        <v>-8.6215785416990727</v>
+        <v>-4.3091230759176486</v>
       </c>
       <c r="K175">
         <v>0.36213927762322257</v>
@@ -7624,7 +7624,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M175">
-        <v>-15.697084614616861</v>
+        <v>-16.434185094589779</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -7656,7 +7656,7 @@
         <v>-0.10905999999999999</v>
       </c>
       <c r="J176">
-        <v>-6.6779220391633567</v>
+        <v>-2.5835940737250676</v>
       </c>
       <c r="K176">
         <v>0.50556835392022581</v>
@@ -7665,7 +7665,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M176">
-        <v>-7.4219152007618536</v>
+        <v>-8.7766903415941169</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
@@ -7697,7 +7697,7 @@
         <v>-0.12041999999999997</v>
       </c>
       <c r="J177">
-        <v>-6.9054958750329885</v>
+        <v>-2.5835940737250676</v>
       </c>
       <c r="K177">
         <v>0.50556835392022581</v>
@@ -7706,7 +7706,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M177">
-        <v>-8.1950030118810027</v>
+        <v>-8.7766903415941169</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
@@ -7738,7 +7738,7 @@
         <v>-0.16596</v>
       </c>
       <c r="J178">
-        <v>-7.8177945093202279</v>
+        <v>-2.5835940737250676</v>
       </c>
       <c r="K178">
         <v>0.50556835392022581</v>
@@ -7747,7 +7747,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M178">
-        <v>-11.294159606807604</v>
+        <v>-8.7766903415941169</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
@@ -7820,7 +7820,7 @@
         <v>-0.12042999999999998</v>
       </c>
       <c r="J180">
-        <v>-6.905696204113859</v>
+        <v>-2.5835940737250676</v>
       </c>
       <c r="K180">
         <v>0.50556835392022581</v>
@@ -7829,7 +7829,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M180">
-        <v>-8.1956835469260039</v>
+        <v>-8.7766903415941169</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
@@ -7861,7 +7861,7 @@
         <v>-0.47929999999999984</v>
       </c>
       <c r="J181">
-        <v>-1.2599140760019483</v>
+        <v>-0.9369411439781089</v>
       </c>
       <c r="K181">
         <v>7.3856895969626177E-2</v>
@@ -7870,7 +7870,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M181">
-        <v>-4.0165736886824543</v>
+        <v>-4.2260757588202837</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
@@ -7902,7 +7902,7 @@
         <v>-0.54739999999999966</v>
       </c>
       <c r="J182">
-        <v>-1.3864373595730548</v>
+        <v>-0.9369411439781089</v>
       </c>
       <c r="K182">
         <v>7.3856895969626177E-2</v>
@@ -7911,7 +7911,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M182">
-        <v>-4.5872573277378992</v>
+        <v>-4.2260757588202837</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -7943,7 +7943,7 @@
         <v>-0.46789999999999976</v>
       </c>
       <c r="J183">
-        <v>-1.2387339668578861</v>
+        <v>-0.9369411439781089</v>
       </c>
       <c r="K183">
         <v>7.3856895969626177E-2</v>
@@ -7952,7 +7952,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M183">
-        <v>-3.9210407446996034</v>
+        <v>-4.2260757588202837</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -7984,7 +7984,7 @@
         <v>-0.5477000000000003</v>
       </c>
       <c r="J184">
-        <v>-1.3869947308663206</v>
+        <v>-0.9369411439781089</v>
       </c>
       <c r="K184">
         <v>7.3856895969626177E-2</v>
@@ -7993,7 +7993,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M184">
-        <v>-4.5897713525795574</v>
+        <v>-4.2260757588202837</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
@@ -8025,7 +8025,7 @@
         <v>-0.47920000000000007</v>
       </c>
       <c r="J185">
-        <v>-1.2597282855708605</v>
+        <v>-0.9369411439781089</v>
       </c>
       <c r="K185">
         <v>7.3856895969626177E-2</v>
@@ -8034,7 +8034,7 @@
         <v>3.8133220027560767E-3</v>
       </c>
       <c r="M185">
-        <v>-4.0157356804019049</v>
+        <v>-4.2260757588202837</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
@@ -8066,7 +8066,7 @@
         <v>-0.3404999999999998</v>
       </c>
       <c r="J186">
-        <v>-1.2630748062592376</v>
+        <v>-0.83427904849671519</v>
       </c>
       <c r="K186">
         <v>7.7684182224272147E-2</v>
@@ -8075,7 +8075,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M186">
-        <v>-3.8775377625928376</v>
+        <v>-3.6136625701222416</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
@@ -8107,7 +8107,7 @@
         <v>-0.28359999999999985</v>
       </c>
       <c r="J187">
-        <v>-1.1421091066461679</v>
+        <v>-0.83427904849671519</v>
       </c>
       <c r="K187">
         <v>7.7684182224272147E-2</v>
@@ -8116,7 +8116,7 @@
         <v>3.9809345132465349E-3</v>
       </c>
       <c r="M187">
-        <v>-3.338473241798205</v>
+        <v>-3.6136625701222416</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
@@ -8148,7 +8148,7 @@
         <v>-0.3176000000000001</v>
       </c>
       <c r="J188">
-        <v>-1.2029729481035545</v>
+        <v>-0.83427904849671519</v>
       </c>
       <c r="K188">
         <v>7.7684182224272147E-2</v>
@@ -8157,7 +8157,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M188">
-        <v>-3.6167576898663323</v>
+        <v>-3.6136625701222416</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -8189,7 +8189,7 @@
         <v>-0.28350000000000009</v>
       </c>
       <c r="J189">
-        <v>-1.1134762946926891</v>
+        <v>-0.83427904849671519</v>
       </c>
       <c r="K189">
         <v>7.7684182224272147E-2</v>
@@ -8198,7 +8198,7 @@
         <v>3.9640757419448346E-3</v>
       </c>
       <c r="M189">
-        <v>-3.2284345248019681</v>
+        <v>-3.6136625701222416</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -8230,7 +8230,7 @@
         <v>-0.34039999999999981</v>
       </c>
       <c r="J190">
-        <v>-1.2968647857614533</v>
+        <v>-0.83427904849671519</v>
       </c>
       <c r="K190">
         <v>7.7684182224272147E-2</v>
@@ -8239,7 +8239,7 @@
         <v>3.9809345132465349E-3</v>
       </c>
       <c r="M190">
-        <v>-4.0071096315518648</v>
+        <v>-3.6136625701222416</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
@@ -8271,7 +8271,7 @@
         <v>-0.21419999999999995</v>
       </c>
       <c r="J191">
-        <v>-1.0973932250873546</v>
+        <v>-0.66618676830452805</v>
       </c>
       <c r="K191">
         <v>0.14355577603806122</v>
@@ -8280,7 +8280,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M191">
-        <v>-3.0668112046870406</v>
+        <v>-2.8065188251295692</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
@@ -8312,7 +8312,7 @@
         <v>-0.13460000000000005</v>
       </c>
       <c r="J192">
-        <v>-0.82686742793889856</v>
+        <v>-0.66618676830452805</v>
       </c>
       <c r="K192">
         <v>0.14355577603806122</v>
@@ -8321,7 +8321,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M192">
-        <v>-1.9271371995839215</v>
+        <v>-2.8065188251295692</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
@@ -8353,7 +8353,7 @@
         <v>-0.24829999999999997</v>
       </c>
       <c r="J193">
-        <v>-1.2132843015039674</v>
+        <v>-0.66618676830452805</v>
       </c>
       <c r="K193">
         <v>0.14355577603806122</v>
@@ -8362,7 +8362,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M193">
-        <v>-3.5550383852651364</v>
+        <v>-2.8065188251295692</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
@@ -8394,7 +8394,7 @@
         <v>-0.18009999999999993</v>
       </c>
       <c r="J194">
-        <v>-0.98150214867074181</v>
+        <v>-0.66618676830452805</v>
       </c>
       <c r="K194">
         <v>0.14355577603806122</v>
@@ -8403,7 +8403,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M194">
-        <v>-2.5785840241089444</v>
+        <v>-2.8065188251295692</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
@@ -8435,7 +8435,7 @@
         <v>-0.20289999999999986</v>
       </c>
       <c r="J195">
-        <v>-1.0589894373012041</v>
+        <v>-0.66618676830452805</v>
       </c>
       <c r="K195">
         <v>0.14355577603806122</v>
@@ -8444,7 +8444,7 @@
         <v>4.0827848052324683E-3</v>
       </c>
       <c r="M195">
-        <v>-2.9050233120028022</v>
+        <v>-2.8065188251295692</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
@@ -8476,7 +8476,7 @@
         <v>-9.8980000000000068E-2</v>
       </c>
       <c r="J196">
-        <v>-0.91735554816988363</v>
+        <v>-0.47695306441767499</v>
       </c>
       <c r="K196">
         <v>0.10492998238437413</v>
@@ -8485,7 +8485,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M196">
-        <v>-2.1806338368907232</v>
+        <v>-1.8957763118267272</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
@@ -8517,7 +8517,7 @@
         <v>-8.7579999999999991E-2</v>
       </c>
       <c r="J197">
-        <v>-0.85424725260044154</v>
+        <v>-0.47695306441767499</v>
       </c>
       <c r="K197">
         <v>0.10492998238437413</v>
@@ -8526,7 +8526,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M197">
-        <v>-1.9294798083945184</v>
+        <v>-1.8957763118267272</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
@@ -8558,7 +8558,7 @@
         <v>-8.7480000000000002E-2</v>
       </c>
       <c r="J198">
-        <v>-0.87826409700561814</v>
+        <v>-0.47695306441767499</v>
       </c>
       <c r="K198">
         <v>0.10492998238437413</v>
@@ -8567,7 +8567,7 @@
         <v>4.3473233346519764E-3</v>
       </c>
       <c r="M198">
-        <v>-2.0132179068083302</v>
+        <v>-1.8957763118267272</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
@@ -8599,7 +8599,7 @@
         <v>-5.3379999999999983E-2</v>
       </c>
       <c r="J199">
-        <v>-0.66492236589211595</v>
+        <v>-0.47695306441767499</v>
       </c>
       <c r="K199">
         <v>0.10492998238437413</v>
@@ -8608,7 +8608,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M199">
-        <v>-1.1760177229059072</v>
+        <v>-1.8957763118267272</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
@@ -8640,7 +8640,7 @@
         <v>-9.8929999999999962E-2</v>
       </c>
       <c r="J200">
-        <v>-0.91707875739984179</v>
+        <v>-0.47695306441767499</v>
       </c>
       <c r="K200">
         <v>0.10492998238437413</v>
@@ -8649,7 +8649,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M200">
-        <v>-2.1795322841341589</v>
+        <v>-1.8957763118267272</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
@@ -8681,7 +8681,7 @@
         <v>-1.8280000000000018E-2</v>
       </c>
       <c r="J201">
-        <v>-0.52677002175965848</v>
+        <v>-0.18989617649656507</v>
       </c>
       <c r="K201">
         <v>0.10267768464039581</v>
@@ -8690,7 +8690,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M201">
-        <v>-0.59392549862764665</v>
+        <v>-0.71994818540859351</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
@@ -8722,7 +8722,7 @@
         <v>-7.0000000000000062E-3</v>
       </c>
       <c r="J202">
-        <v>-0.42967471779077793</v>
+        <v>-0.18989617649656507</v>
       </c>
       <c r="K202">
         <v>0.10267768464039581</v>
@@ -8731,7 +8731,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M202">
-        <v>-0.227433177811462</v>
+        <v>-0.71994818540859351</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
@@ -8763,7 +8763,7 @@
         <v>-1.8280000000000018E-2</v>
       </c>
       <c r="J203">
-        <v>-0.52677002175965848</v>
+        <v>-0.18989617649656507</v>
       </c>
       <c r="K203">
         <v>0.10267768464039581</v>
@@ -8772,7 +8772,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M203">
-        <v>-0.59392549862764665</v>
+        <v>-0.71994818540859351</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
@@ -8804,7 +8804,7 @@
         <v>-2.9730000000000034E-2</v>
       </c>
       <c r="J204">
-        <v>-0.6104012074999412</v>
+        <v>-0.18989617649656507</v>
       </c>
       <c r="K204">
         <v>0.10267768464039581</v>
@@ -8813,7 +8813,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M204">
-        <v>-0.91625140006000005</v>
+        <v>-0.71994818540859351</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
@@ -8845,7 +8845,7 @@
         <v>-4.115000000000002E-2</v>
       </c>
       <c r="J205">
-        <v>-0.70296761265231544</v>
+        <v>-0.18989617649656507</v>
       </c>
       <c r="K205">
         <v>0.10267768464039581</v>
@@ -8854,7 +8854,7 @@
         <v>4.5237229479136356E-3</v>
       </c>
       <c r="M205">
-        <v>-1.268205351916212</v>
+        <v>-0.71994818540859351</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
@@ -8886,7 +8886,7 @@
         <v>6.2200000000000005E-2</v>
       </c>
       <c r="J206">
-        <v>0.76836093930811256</v>
+        <v>0.88773296291816095</v>
       </c>
       <c r="K206">
         <v>0.2714073177833366</v>
@@ -8895,7 +8895,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M206">
-        <v>3.9102700145699516</v>
+        <v>3.0509158828791891</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
@@ -8927,7 +8927,7 @@
         <v>3.9377000000000002E-2</v>
       </c>
       <c r="J207">
-        <v>0.35087562262658528</v>
+        <v>0.88773296291816095</v>
       </c>
       <c r="K207">
         <v>0.2714073177833366</v>
@@ -8936,7 +8936,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M207">
-        <v>2.47547752996336</v>
+        <v>3.0509158828791891</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
@@ -8968,7 +8968,7 @@
         <v>5.0824999999999995E-2</v>
       </c>
       <c r="J208">
-        <v>0.56028595016328597</v>
+        <v>0.88773296291816095</v>
       </c>
       <c r="K208">
         <v>0.2714073177833366</v>
@@ -8977,7 +8977,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M208">
-        <v>3.1951683840919256</v>
+        <v>3.0509158828791891</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
@@ -9009,7 +9009,7 @@
         <v>2.8074000000000002E-2</v>
       </c>
       <c r="J209">
-        <v>0.14411767956689542</v>
+        <v>0.88773296291816095</v>
       </c>
       <c r="K209">
         <v>0.2714073177833366</v>
@@ -9018,7 +9018,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M209">
-        <v>1.7649022570584703</v>
+        <v>3.0509158828791891</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>6.2176000000000002E-2</v>
       </c>
       <c r="J210">
-        <v>0.76792192394640035</v>
+        <v>0.88773296291816095</v>
       </c>
       <c r="K210">
         <v>0.2714073177833366</v>
@@ -9059,7 +9059,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M210">
-        <v>3.90876122871224</v>
+        <v>3.0509158828791891</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
@@ -9091,7 +9091,7 @@
         <v>8.6455000000000002</v>
       </c>
       <c r="J211">
-        <v>65.86137489647092</v>
+        <v>32.651667131565134</v>
       </c>
       <c r="K211">
         <v>0.44665280978676947</v>
@@ -9100,7 +9100,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M211">
-        <v>137.94279057667458</v>
+        <v>135.6248634584019</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
@@ -9132,7 +9132,7 @@
         <v>8.4062999999999999</v>
       </c>
       <c r="J212">
-        <v>64.942542891686287</v>
+        <v>32.651667131565134</v>
       </c>
       <c r="K212">
         <v>0.44665280978676947</v>
@@ -9141,7 +9141,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M212">
-        <v>134.12624838640903</v>
+        <v>135.6248634584019</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
@@ -9173,7 +9173,7 @@
         <v>8.4063000000000017</v>
       </c>
       <c r="J213">
-        <v>64.942542891686315</v>
+        <v>32.651667131565134</v>
       </c>
       <c r="K213">
         <v>0.44665280978676947</v>
@@ -9182,7 +9182,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M213">
-        <v>134.12624838640909</v>
+        <v>135.6248634584019</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
@@ -9214,7 +9214,7 @@
         <v>8.5428000000000015</v>
       </c>
       <c r="J214">
-        <v>65.466876372677518</v>
+        <v>32.651667131565134</v>
       </c>
       <c r="K214">
         <v>0.44665280978676947</v>
@@ -9223,7 +9223,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M214">
-        <v>136.30416648411494</v>
+        <v>135.6248634584019</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
@@ -9255,7 +9255,7 @@
         <v>8.4063999999999997</v>
       </c>
       <c r="J215">
-        <v>73.832675289987293</v>
+        <v>32.276964448456361</v>
       </c>
       <c r="K215">
         <v>0.52521975547483457</v>
@@ -9264,7 +9264,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M215">
-        <v>134.12784393080295</v>
+        <v>134.20275245525841</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
@@ -9296,7 +9296,7 @@
         <v>8.4859999999999989</v>
       </c>
       <c r="J216">
-        <v>74.138440455459104</v>
+        <v>32.276964448456361</v>
       </c>
       <c r="K216">
         <v>0.52521975547483457</v>
@@ -9305,7 +9305,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M216">
-        <v>135.39789726836622</v>
+        <v>134.20275245525841</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
@@ -9337,7 +9337,7 @@
         <v>8.5428000000000015</v>
       </c>
       <c r="J217">
-        <v>74.356624643886221</v>
+        <v>32.276964448456361</v>
       </c>
       <c r="K217">
         <v>0.52521975547483457</v>
@@ -9346,7 +9346,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M217">
-        <v>136.30416648411494</v>
+        <v>134.20275245525841</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
@@ -9378,7 +9378,7 @@
         <v>8.3948999999999998</v>
       </c>
       <c r="J218">
-        <v>73.788500674372656</v>
+        <v>32.276964448456361</v>
       </c>
       <c r="K218">
         <v>0.52521975547483457</v>
@@ -9387,7 +9387,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M218">
-        <v>133.94435632550176</v>
+        <v>134.20275245525841</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
@@ -9419,7 +9419,7 @@
         <v>8.5542999999999996</v>
       </c>
       <c r="J219">
-        <v>72.975658192445678</v>
+        <v>32.276964448456361</v>
       </c>
       <c r="K219">
         <v>0.52521975547483457</v>
@@ -9428,7 +9428,7 @@
         <v>4.1197123055157318E-3</v>
       </c>
       <c r="M219">
-        <v>131.23949826750615</v>
+        <v>134.20275245525841</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
@@ -9460,7 +9460,7 @@
         <v>6.3093000000000004</v>
       </c>
       <c r="J220">
-        <v>76.468535511219386</v>
+        <v>33.208017365207311</v>
       </c>
       <c r="K220">
         <v>1.0621485409254601</v>
@@ -9469,7 +9469,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M220">
-        <v>139.00053613956996</v>
+        <v>132.8153333467871</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.25">
@@ -9501,7 +9501,7 @@
         <v>6.1271000000000004</v>
       </c>
       <c r="J221">
-        <v>73.706885221969273</v>
+        <v>33.208017365207311</v>
       </c>
       <c r="K221">
         <v>1.0621485409254601</v>
@@ -9510,7 +9510,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M221">
-        <v>128.81502763789575</v>
+        <v>132.8153333467871</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
@@ -9542,7 +9542,7 @@
         <v>6.1952999999999996</v>
       </c>
       <c r="J222">
-        <v>74.064915128722731</v>
+        <v>33.208017365207311</v>
       </c>
       <c r="K222">
         <v>1.0621485409254601</v>
@@ -9551,7 +9551,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M222">
-        <v>130.24885194056819</v>
+        <v>132.8153333467871</v>
       </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.25">
@@ -9583,7 +9583,7 @@
         <v>6.3207000000000004</v>
       </c>
       <c r="J223">
-        <v>74.723228183075861</v>
+        <v>33.208017365207311</v>
       </c>
       <c r="K223">
         <v>1.0621485409254601</v>
@@ -9592,7 +9592,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M223">
-        <v>132.88523856161112</v>
+        <v>132.8153333467871</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.25">
@@ -9624,7 +9624,7 @@
         <v>6.3321999999999985</v>
       </c>
       <c r="J224">
-        <v>74.783599794918445</v>
+        <v>33.208017365207311</v>
       </c>
       <c r="K224">
         <v>1.0621485409254601</v>
@@ -9633,7 +9633,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M224">
-        <v>133.12701245429048</v>
+        <v>132.8153333467871</v>
       </c>
     </row>
     <row r="225" spans="1:13" x14ac:dyDescent="0.25">
@@ -9665,7 +9665,7 @@
         <v>4.1091999999999995</v>
       </c>
       <c r="J225">
-        <v>76.912339433706777</v>
+        <v>37.367231877881999</v>
       </c>
       <c r="K225">
         <v>1.6251474792105427</v>
@@ -9674,7 +9674,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M225">
-        <v>133.50977346612271</v>
+        <v>140.32318375288554</v>
       </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.25">
@@ -9706,7 +9706,7 @@
         <v>4.1663000000000006</v>
       </c>
       <c r="J226">
-        <v>79.93530478634456</v>
+        <v>37.367231877881999</v>
       </c>
       <c r="K226">
         <v>1.6251474792105427</v>
@@ -9715,7 +9715,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M226">
-        <v>143.72156335781668</v>
+        <v>140.32318375288554</v>
       </c>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.25">
@@ -9747,7 +9747,7 @@
         <v>4.1549000000000005</v>
       </c>
       <c r="J227">
-        <v>79.830249860157608</v>
+        <v>37.367231877881999</v>
       </c>
       <c r="K227">
         <v>1.6251474792105427</v>
@@ -9756,7 +9756,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M227">
-        <v>143.32830655387093</v>
+        <v>140.32318375288554</v>
       </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.25">
@@ -9788,7 +9788,7 @@
         <v>4.1663000000000006</v>
       </c>
       <c r="J228">
-        <v>77.403841371350666</v>
+        <v>37.367231877881999</v>
       </c>
       <c r="K228">
         <v>1.6251474792105427</v>
@@ -9797,7 +9797,7 @@
         <v>4.5568191566621096E-3</v>
       </c>
       <c r="M228">
-        <v>135.36497838798482</v>
+        <v>140.32318375288554</v>
       </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.25">
@@ -9829,7 +9829,7 @@
         <v>4.2233999999999998</v>
       </c>
       <c r="J229">
-        <v>80.461500951719557</v>
+        <v>37.367231877881999</v>
       </c>
       <c r="K229">
         <v>1.6251474792105427</v>
@@ -9838,7 +9838,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M229">
-        <v>145.69129699863259</v>
+        <v>140.32318375288554</v>
       </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.25">
@@ -9993,7 +9993,7 @@
         <v>2.0916999999999999</v>
       </c>
       <c r="J233">
-        <v>83.444249248593323</v>
+        <v>41.902833845819487</v>
       </c>
       <c r="K233">
         <v>0</v>
@@ -10280,7 +10280,7 @@
         <v>-1.8245999999999998</v>
       </c>
       <c r="J240">
-        <v>-11.620582193180867</v>
+        <v>-6.8991146412768529</v>
       </c>
       <c r="K240">
         <v>0.261116495183561</v>
@@ -10289,7 +10289,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M240">
-        <v>-29.112303011532056</v>
+        <v>-28.656775087066841</v>
       </c>
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.25">
@@ -10321,7 +10321,7 @@
         <v>-1.8699999999999997</v>
       </c>
       <c r="J241">
-        <v>-11.794975893085642</v>
+        <v>-6.8991146412768529</v>
       </c>
       <c r="K241">
         <v>0.261116495183561</v>
@@ -10330,7 +10330,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M241">
-        <v>-29.836680166373419</v>
+        <v>-28.656775087066841</v>
       </c>
     </row>
     <row r="242" spans="1:13" x14ac:dyDescent="0.25">
@@ -10362,7 +10362,7 @@
         <v>-1.7107000000000001</v>
       </c>
       <c r="J242">
-        <v>-11.183061435049728</v>
+        <v>-6.8991146412768529</v>
       </c>
       <c r="K242">
         <v>0.261116495183561</v>
@@ -10371,7 +10371,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M242">
-        <v>-27.294977946852949</v>
+        <v>-28.656775087066841</v>
       </c>
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.25">
@@ -10403,7 +10403,7 @@
         <v>-1.7789000000000001</v>
       </c>
       <c r="J243">
-        <v>-11.44503611199919</v>
+        <v>-6.8991146412768529</v>
       </c>
       <c r="K243">
         <v>0.261116495183561</v>
@@ -10412,7 +10412,7 @@
         <v>4.14089762261898E-3</v>
       </c>
       <c r="M243">
-        <v>-28.383139223508927</v>
+        <v>-28.656775087066841</v>
       </c>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.25">
@@ -10485,7 +10485,7 @@
         <v>-1.31</v>
       </c>
       <c r="J245">
-        <v>-11.488913311729913</v>
+        <v>-6.7568494587994818</v>
       </c>
       <c r="K245">
         <v>0.36352878041927095</v>
@@ -10494,7 +10494,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M245">
-        <v>-27.541199948694064</v>
+        <v>-26.95570698991515</v>
       </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.25">
@@ -10526,7 +10526,7 @@
         <v>-1.2075</v>
       </c>
       <c r="J246">
-        <v>-11.296296363552091</v>
+        <v>-6.7568494587994818</v>
       </c>
       <c r="K246">
         <v>0.36352878041927095</v>
@@ -10535,7 +10535,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M246">
-        <v>-26.602499070979459</v>
+        <v>-26.95570698991515</v>
       </c>
     </row>
     <row r="247" spans="1:13" x14ac:dyDescent="0.25">
@@ -10567,7 +10567,7 @@
         <v>-1.2644000000000002</v>
       </c>
       <c r="J247">
-        <v>-11.611284259859218</v>
+        <v>-6.7568494587994818</v>
       </c>
       <c r="K247">
         <v>0.36352878041927095</v>
@@ -10576,7 +10576,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M247">
-        <v>-27.856066107947356</v>
+        <v>-26.95570698991515</v>
       </c>
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.25">
@@ -10608,7 +10608,7 @@
         <v>-1.1734</v>
       </c>
       <c r="J248">
-        <v>-10.771803557147468</v>
+        <v>-6.7568494587994818</v>
       </c>
       <c r="K248">
         <v>0.36352878041927095</v>
@@ -10617,7 +10617,7 @@
         <v>4.2948877241664584E-3</v>
       </c>
       <c r="M248">
-        <v>-24.669346579998184</v>
+        <v>-26.95570698991515</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
@@ -10649,7 +10649,7 @@
         <v>-1.2759</v>
       </c>
       <c r="J249">
-        <v>-11.674946136968742</v>
+        <v>-6.7568494587994818</v>
       </c>
       <c r="K249">
         <v>0.36352878041927095</v>
@@ -10658,7 +10658,7 @@
         <v>4.3219003505285481E-3</v>
       </c>
       <c r="M249">
-        <v>-28.109423241956684</v>
+        <v>-26.95570698991515</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.25">
@@ -10690,7 +10690,7 @@
         <v>-0.60189999999999988</v>
       </c>
       <c r="J250">
-        <v>-10.158515062835123</v>
+        <v>-5.9469752687969955</v>
       </c>
       <c r="K250">
         <v>0.39504171195144128</v>
@@ -10699,7 +10699,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M250">
-        <v>-20.763269324117285</v>
+        <v>-22.191174627080944</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.25">
@@ -10731,7 +10731,7 @@
         <v>-0.62449999999999983</v>
       </c>
       <c r="J251">
-        <v>-10.366781846328557</v>
+        <v>-5.9469752687969955</v>
       </c>
       <c r="K251">
         <v>0.39504171195144128</v>
@@ -10740,7 +10740,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M251">
-        <v>-21.542883689834262</v>
+        <v>-22.191174627080944</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.25">
@@ -10772,7 +10772,7 @@
         <v>-0.64729999999999999</v>
       </c>
       <c r="J252">
-        <v>-10.971695362845441</v>
+        <v>-5.9469752687969955</v>
       </c>
       <c r="K252">
         <v>0.39504171195144128</v>
@@ -10781,7 +10781,7 @@
         <v>4.6309623890744174E-3</v>
       </c>
       <c r="M252">
-        <v>-23.621485915265829</v>
+        <v>-22.191174627080944</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.25">
@@ -10813,7 +10813,7 @@
         <v>-0.69269999999999987</v>
       </c>
       <c r="J253">
-        <v>-10.995268334569808</v>
+        <v>-5.9469752687969955</v>
       </c>
       <c r="K253">
         <v>0.39504171195144128</v>
@@ -10822,7 +10822,7 @@
         <v>4.594821277815582E-3</v>
       </c>
       <c r="M253">
-        <v>-23.895525271334183</v>
+        <v>-22.191174627080944</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.25">
@@ -10854,7 +10854,7 @@
         <v>-0.57910000000000017</v>
       </c>
       <c r="J254">
-        <v>-10.301612072666064</v>
+        <v>-5.9469752687969955</v>
       </c>
       <c r="K254">
         <v>0.39504171195144128</v>
@@ -10863,7 +10863,7 @@
         <v>4.6309623890744174E-3</v>
       </c>
       <c r="M254">
-        <v>-21.132708934853152</v>
+        <v>-22.191174627080944</v>
       </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.25">
@@ -10895,7 +10895,7 @@
         <v>-0.24707999999999997</v>
       </c>
       <c r="J255">
-        <v>-9.5615301972164986</v>
+        <v>-4.3308572022839389</v>
       </c>
       <c r="K255">
         <v>0.51033911932080656</v>
@@ -10904,7 +10904,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M255">
-        <v>-16.81465989184154</v>
+        <v>-14.741526484057227</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.25">
@@ -10936,7 +10936,7 @@
         <v>-0.2355600000000001</v>
       </c>
       <c r="J256">
-        <v>-9.3307510960529321</v>
+        <v>-4.3308572022839389</v>
       </c>
       <c r="K256">
         <v>0.51033911932080656</v>
@@ -10945,7 +10945,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M256">
-        <v>-16.030683520002412</v>
+        <v>-14.741526484057227</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
@@ -10977,7 +10977,7 @@
         <v>-0.20147999999999999</v>
       </c>
       <c r="J257">
-        <v>-8.6480295884440341</v>
+        <v>-4.3308572022839389</v>
       </c>
       <c r="K257">
         <v>0.51033911932080656</v>
@@ -10986,7 +10986,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M257">
-        <v>-13.711420086644953</v>
+        <v>-14.741526484057227</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
         <v>-0.21285999999999994</v>
       </c>
       <c r="J258">
-        <v>-8.8760040824754078</v>
+        <v>-4.3308572022839389</v>
       </c>
       <c r="K258">
         <v>0.51033911932080656</v>
@@ -11027,7 +11027,7 @@
         <v>5.063163486294299E-3</v>
       </c>
       <c r="M258">
-        <v>-14.485868967854096</v>
+        <v>-14.741526484057227</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.25">
@@ -11059,7 +11059,7 @@
         <v>-0.20145999999999997</v>
       </c>
       <c r="J259">
-        <v>-8.2969673824908359</v>
+        <v>-4.3308572022839389</v>
       </c>
       <c r="K259">
         <v>0.51033911932080656</v>
@@ -11068,7 +11068,7 @@
         <v>5.0047289234938881E-3</v>
       </c>
       <c r="M259">
-        <v>-12.664999953943127</v>
+        <v>-14.741526484057227</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>